<commit_message>
Se crea un repaldo de la maquina funcionando, pero el verdaderop es el 10, que realiza los flejes bien
</commit_message>
<xml_diff>
--- a/Libro de Contantes.xlsx
+++ b/Libro de Contantes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\FlejadoraAutomatica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32FBEAC4-6268-4E3F-BF17-433321ABBF8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86AFBDF-4351-4E58-A100-7BCC5ECAE8AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{6CDE3574-5F0F-43AB-BDDA-685E75322216}"/>
+    <workbookView xWindow="825" yWindow="-120" windowWidth="19785" windowHeight="11760" activeTab="1" xr2:uid="{6CDE3574-5F0F-43AB-BDDA-685E75322216}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -2528,16 +2528,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2864,8 +2864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04924357-64FA-48BF-BCE9-EF47D2829CDA}">
   <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3247,8 +3247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{142EE1C5-4986-4428-8B1E-A4C37DA95A3B}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>